<commit_message>
:sparkles: Criando report anual
</commit_message>
<xml_diff>
--- a/GenerateYearlyReportExecutor/Data/Config.xlsx
+++ b/GenerateYearlyReportExecutor/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Documents\GitHub\UiPath\GenerateYearlyReportExecutor\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F28F03C-B3E5-41FF-B07B-56BDA47DC8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CBCB9C-B043-4CE9-8C2C-4F7E51EAC4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4560" yWindow="1785" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>https://acme-test.uipath.com/login</t>
+  </si>
+  <si>
+    <t>DownloadFolder</t>
+  </si>
+  <si>
+    <t>Data\Temp</t>
   </si>
 </sst>
 </file>
@@ -561,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -658,7 +664,14 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
:sparkles: Atualizando report anual
</commit_message>
<xml_diff>
--- a/GenerateYearlyReportExecutor/Data/Config.xlsx
+++ b/GenerateYearlyReportExecutor/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Documents\GitHub\UiPath\GenerateYearlyReportExecutor\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CBCB9C-B043-4CE9-8C2C-4F7E51EAC4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C421346-4A25-40F4-A172-04C930026EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="1785" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -568,7 +568,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>